<commit_message>
more historic photos added
</commit_message>
<xml_diff>
--- a/images/Image_Map_Log.xlsx
+++ b/images/Image_Map_Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\GIS\GIS_Work\JFreeman\Personal\MAP698\Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfr236\Desktop\MAP698\uky-history-ownership\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FA2722-41D2-48C2-AC7D-46A80EEE0331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C260652C-EC02-4A06-8C29-3757C94DBCC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32820" yWindow="2445" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Images" sheetId="2" r:id="rId4"/>
     <sheet name="Text" sheetId="3" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Maps!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="334">
   <si>
     <t>https://exploreuk.uky.edu/catalog/xt7pzg6g4p2j?f%5Bformat%5D%5B%5D=maps&amp;f%5Bsource_s%5D%5B%5D=University+of+Kentucky+campus+maps+and+guidebooks+collection&amp;per_page=20#page/1/mode/1up</t>
   </si>
@@ -541,15 +544,6 @@
     <t>C:\Users\jmfr236\Desktop\MAP698\uky-parcel-ownership\images\historic\1909_experiment_station.jpg</t>
   </si>
   <si>
-    <t>C:\Users\jmfr236\Desktop\MAP698\uky-parcel-ownership\images\historic\vivarium_experiement_station.jpg</t>
-  </si>
-  <si>
-    <t>https://exploreuk.uky.edu/catalog/xt702v2c8b60_1_15?q=Agricultural+Experiment+Station&amp;per_page=20</t>
-  </si>
-  <si>
-    <t>Vivarium</t>
-  </si>
-  <si>
     <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_20_4?q=Agricultural+Experiment+Station&amp;per_page=20</t>
   </si>
   <si>
@@ -721,12 +715,6 @@
     <t>American Tobacco Company SAVS</t>
   </si>
   <si>
-    <t>https://exploreuk.uky.edu/catalog/xt702v2c8b60_1_437?q=experiment+station&amp;f%5Bformat%5D%5B%5D=images&amp;offset=180&amp;per_page=20</t>
-  </si>
-  <si>
-    <t>experiment station Pond</t>
-  </si>
-  <si>
     <t>Main Building Back</t>
   </si>
   <si>
@@ -769,15 +757,6 @@
     <t>Myrtle Weldon</t>
   </si>
   <si>
-    <t>Maxwell Place</t>
-  </si>
-  <si>
-    <t>Gillis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Margaret I. King </t>
-  </si>
-  <si>
     <t>Drawing</t>
   </si>
   <si>
@@ -830,13 +809,238 @@
   </si>
   <si>
     <t>memorial colesium and stoll field</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>maxwell Place</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_69_5?q=maxwell+place&amp;f%5Bformat%5D%5B%5D=images&amp;offset=60&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_2148_1?q=maxwell+place&amp;f%5Bformat%5D%5B%5D=images&amp;offset=100&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7f4q7qpg4w_1_132?q=patterson+house&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_386_29?q=patterson+house&amp;per_page=20; https://exploreuk.uky.edu/catalog/xt75736m0s6q_153_2?q=patterson+house&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_925_1?q=miller+hall&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7p8c9r2s1z_1_6?q=miller+hall&amp;offset=60&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_2117_1?q=miller+hall&amp;offset=60&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7sf7664q86_183_1?q=law+building&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_109_2?q=law+building&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>mathews/ ag</t>
+  </si>
+  <si>
+    <t>gillis / experiment station, law, chemistry</t>
+  </si>
+  <si>
+    <t>chem-phys</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7k0p0wsx4b_95?q=chemistry+building&amp;offset=40&amp;per_page=20#page/1/mode/1up/search/chemistry+building</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_1586_1?q=chemistry+building&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_3642_1?q=chemistry+building&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>funkhouser</t>
+  </si>
+  <si>
+    <t>scovell/ experiment station</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt702v2c8b60_1_1?q=experiment+station+building&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_973_1?q=experiment+station+building&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>laferty/ law</t>
+  </si>
+  <si>
+    <t>pot</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_10_77?q=patterson+office+tower&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_134_12?q=patterson+tower&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_88_1?q=frazee+hall&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>frazee</t>
+  </si>
+  <si>
+    <t>Alumni Hall</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7sf7664q86_395_1?q=frazee+hall&amp;offset=60&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>Bradley Hall/ men dorm</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7sf7664q86_493_1?q=frazee+hall&amp;offset=160&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>Kinkead/ men dorm</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_342_3?q=men+dorm&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_434_1?q=men+dorm&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>neville dorm (demo)</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_279_33?q=dorm&amp;offset=80&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7gqn5z6m6g_14_1?q=library&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_63_7?q=library&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_30_15?q=library&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_76_1?q=neville+hall&amp;f%5Bformat%5D%5B%5D=images&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>taylor ed</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_84_2?q=education+building&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_84_8?q=education+building&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_276_1?q=rose+street&amp;f%5Bformat%5D%5B%5D=images&amp;offset=20&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>University site as it looked in a 1857 pictorial map of Lexington; Limestone is to the left, Rose Street is near the center, and the Fair Amphitheater is in the foreground; Photographer: Lafayette Studio</t>
+  </si>
+  <si>
+    <t>railroad memorial</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_3549_1?q=railroad+memorial&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_1972_1?q=railroad+memorial&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7n8p5v980r_3498_1?q=railroad+memorial&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7sf7664q86_1532_1?q=railroad+memorial&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>carnegie library (demo)</t>
+  </si>
+  <si>
+    <t>Patterson House (demo)</t>
+  </si>
+  <si>
+    <t>Margaret I. King Library</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7sf7664q86_1910_1?q=farm+pre-construction&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>chandler hospital</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_119_81?q=medical+center&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_119_82?q=chandler+med+center&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_28_2?q=johnson+center&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_28_3?q=dairy+center&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_56_2?q=cooper+building&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>Cooper Building</t>
+  </si>
+  <si>
+    <t>McVey/Observatory</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7prr1pgv6h_43_1?q=observatory&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>Donovan</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_69_10?q=donovan+hall&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>Kirwan-Blanding</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt75736m0s6q_63_5?q=kirwan+blanding&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt70cf9j443v_142_1?q=baseball&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt70cf9j443v_125_1?q=baseball&amp;f%5Bformat%5D%5B%5D=images&amp;offset=40&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>https://exploreuk.uky.edu/catalog/xt7sf7664q86_1499_1?q=lake+university&amp;f%5Bformat%5D%5B%5D=images&amp;per_page=20</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>Clifton Pond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,6 +1081,14 @@
       <color rgb="FF333333"/>
       <name val="Proxima-nova"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -905,7 +1117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -922,6 +1134,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1205,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD172F64-40C3-4BA3-BDA5-35E7478C6922}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1353,7 +1568,7 @@
         <v>129</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30">
@@ -1364,7 +1579,7 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30">
@@ -1372,10 +1587,10 @@
         <v>130</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45">
@@ -1383,10 +1598,10 @@
         <v>150</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C22" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1434,7 +1649,7 @@
         <v>134</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30">
@@ -1459,7 +1674,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>106</v>
@@ -1482,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95D705D-2034-4DC6-B002-472F3A5A5E9A}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1507,7 +1722,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s">
         <v>159</v>
@@ -1529,109 +1744,109 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
         <v>172</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
         <v>174</v>
       </c>
-      <c r="B5" t="s">
-        <v>173</v>
-      </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" t="s">
         <v>177</v>
-      </c>
-      <c r="C6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
         <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" t="s">
         <v>187</v>
-      </c>
-      <c r="B10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
         <v>188</v>
-      </c>
-      <c r="C11" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -1639,219 +1854,504 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" t="s">
         <v>198</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" t="s">
         <v>202</v>
-      </c>
-      <c r="B15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C15" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>203</v>
-      </c>
-      <c r="B16" t="s">
-        <v>204</v>
-      </c>
-      <c r="C16" t="s">
-        <v>205</v>
+        <v>210</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>215</v>
+        <v>213</v>
+      </c>
+      <c r="B19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>216</v>
-      </c>
-      <c r="B20" t="s">
-        <v>224</v>
-      </c>
-      <c r="C20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>225</v>
-      </c>
       <c r="B21" t="s">
-        <v>226</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>231</v>
-      </c>
       <c r="B22" t="s">
-        <v>230</v>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B27" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B28" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>222</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>252</v>
+      </c>
+      <c r="B38" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>244</v>
+      <c r="B39" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>245</v>
+        <v>256</v>
+      </c>
+      <c r="B40" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>246</v>
+        <v>262</v>
+      </c>
+      <c r="B41" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>247</v>
+      <c r="B42" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>248</v>
+        <v>313</v>
+      </c>
+      <c r="B43" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="B44" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="B45" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>264</v>
-      </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>273</v>
+      </c>
+      <c r="B48" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>272</v>
+      </c>
+      <c r="B50" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>283</v>
+      </c>
+      <c r="B51" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>274</v>
+      </c>
+      <c r="B52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>277</v>
+      </c>
+      <c r="B53" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>279</v>
+      </c>
+      <c r="B54" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>280</v>
+      </c>
+      <c r="B55" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>284</v>
+      </c>
+      <c r="B56" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="B57" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>288</v>
+      </c>
+      <c r="B58" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>289</v>
+      </c>
+      <c r="B59" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>291</v>
+      </c>
+      <c r="B60" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="B61" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>293</v>
+      </c>
+      <c r="B62" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="B64" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>314</v>
+      </c>
+      <c r="B65" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="B66" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>312</v>
+      </c>
+      <c r="B67" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>302</v>
+      </c>
+      <c r="B68" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="B69" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>307</v>
+      </c>
+      <c r="B70" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="B71" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="B72" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="B73" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>316</v>
+      </c>
+      <c r="B74" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="B75" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>322</v>
+      </c>
+      <c r="B76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>323</v>
+      </c>
+      <c r="B77" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>325</v>
+      </c>
+      <c r="B78" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>327</v>
+      </c>
+      <c r="B79" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>234</v>
+      </c>
+      <c r="B80" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="B81" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="B82" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>332</v>
+      </c>
+      <c r="B83" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>333</v>
+      </c>
+      <c r="B84" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="B85" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B49" r:id="rId1" xr:uid="{25338930-C8A2-45AB-B171-40449D724F76}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{0D816669-323E-4E35-92C3-D39CDFE2678C}"/>
+    <hyperlink ref="B81" r:id="rId3" xr:uid="{27D1A5D3-350E-4CBC-A85F-9526B005D480}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1859,185 +2359,212 @@
     <col min="2" max="2" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5">
-      <c r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="47.25">
+      <c r="A2">
+        <v>1862</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="141.75">
+      <c r="A3">
+        <v>1907</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4">
+        <v>1909</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.5">
+      <c r="A5">
         <v>1918</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="31.5">
-      <c r="A2">
-        <v>1957</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="31.5">
-      <c r="A3">
-        <v>1918</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="31.5">
-      <c r="A4">
-        <v>1958</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="63">
-      <c r="A5">
-        <v>1937</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="31.5">
       <c r="A6">
-        <v>1991</v>
+        <v>1918</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.5">
       <c r="A7">
-        <v>1969</v>
+        <v>1918</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="141.75">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="63">
       <c r="A8">
-        <v>1907</v>
+        <v>1937</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.5">
       <c r="A9">
-        <v>1986</v>
+        <v>1950</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>209</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.5">
-      <c r="A10" t="s">
-        <v>227</v>
+      <c r="A10">
+        <v>1957</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="31.5">
       <c r="A11">
-        <v>1909</v>
+        <v>1958</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75">
+      <c r="A12">
+        <v>1969</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.5">
       <c r="A13">
-        <v>1918</v>
+        <v>1986</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="47.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="31.5">
       <c r="A14">
-        <v>1862</v>
+        <v>1991</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.5">
-      <c r="A15">
-        <v>1950</v>
+      <c r="A15" t="s">
+        <v>224</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>212</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>211</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="B16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23.25">
+      <c r="A17">
+        <v>1857</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{3BC59D1A-3FCE-49E5-94B2-0A35D210448A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId4" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C5" r:id="rId5" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C6" r:id="rId6" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C7" r:id="rId7" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C8" r:id="rId8" location="page/79/mode/1up/search/Lexington" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C9" r:id="rId9" location="page/1/mode/1up/search/Lexington" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" location="page/1/mode/1up/search/university+of+kentucky" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId13" location="page/1/mode/1up/search/university+of+kentucky" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C12" r:id="rId14" xr:uid="{1F7127BC-9C01-4098-A671-4FD0F12F6F90}"/>
-    <hyperlink ref="C15" r:id="rId15" location="page/1/mode/1up/search/university+of+kentucky" xr:uid="{ADEB824E-1231-4714-9D36-5FAE2BB5DA05}"/>
+    <hyperlink ref="C5" r:id="rId1" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C10" r:id="rId2" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C6" r:id="rId3" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C11" r:id="rId4" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C8" r:id="rId5" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C14" r:id="rId6" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C12" r:id="rId7" location="page/1/mode/1up" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C3" r:id="rId8" location="page/79/mode/1up/search/Lexington" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C13" r:id="rId9" location="page/1/mode/1up/search/Lexington" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C7" r:id="rId12" location="page/1/mode/1up/search/university+of+kentucky" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C2" r:id="rId13" location="page/1/mode/1up/search/university+of+kentucky" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C16" r:id="rId14" xr:uid="{1F7127BC-9C01-4098-A671-4FD0F12F6F90}"/>
+    <hyperlink ref="C9" r:id="rId15" location="page/1/mode/1up/search/university+of+kentucky" xr:uid="{ADEB824E-1231-4714-9D36-5FAE2BB5DA05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
@@ -2048,18 +2575,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47.25">
+    <row r="1" spans="1:3" ht="31.5">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -2070,7 +2597,7 @@
     </row>
     <row r="2" spans="1:3" ht="31.5">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -2081,7 +2608,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>24</v>
@@ -2092,7 +2619,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
@@ -2101,9 +2628,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="78.75">
+    <row r="5" spans="1:3" ht="47.25">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>28</v>
@@ -2114,7 +2641,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>30</v>
@@ -2123,9 +2650,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>32</v>
@@ -2134,9 +2661,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25">
+    <row r="8" spans="1:3" ht="31.5">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
@@ -2145,9 +2672,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="78.75">
+    <row r="9" spans="1:3" ht="47.25">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>36</v>
@@ -2158,7 +2685,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>38</v>
@@ -2169,7 +2696,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75">
       <c r="A11" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>40</v>
@@ -2178,9 +2705,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="126">
+    <row r="12" spans="1:3" ht="63">
       <c r="A12" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>41</v>
@@ -2191,7 +2718,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>44</v>
@@ -2202,7 +2729,7 @@
     </row>
     <row r="14" spans="1:3" ht="31.5">
       <c r="A14" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>46</v>
@@ -2211,9 +2738,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5">
+    <row r="15" spans="1:3" ht="15.75">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>48</v>
@@ -2222,9 +2749,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.5">
+    <row r="16" spans="1:3" ht="15.75">
       <c r="A16" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>50</v>
@@ -2235,7 +2762,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75">
       <c r="A17" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>52</v>
@@ -2244,9 +2771,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="47.25">
+    <row r="18" spans="1:3" ht="31.5">
       <c r="A18" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>54</v>
@@ -2257,7 +2784,7 @@
     </row>
     <row r="19" spans="1:3" ht="31.5">
       <c r="A19" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>56</v>
@@ -2266,9 +2793,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.5">
+    <row r="20" spans="1:3" ht="15.75">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>58</v>
@@ -2277,9 +2804,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="78.75">
+    <row r="21" spans="1:3" ht="47.25">
       <c r="A21" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>62</v>
@@ -2288,9 +2815,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="78.75">
+    <row r="22" spans="1:3" ht="47.25">
       <c r="A22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>64</v>
@@ -2299,9 +2826,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="63">
+    <row r="23" spans="1:3" ht="31.5">
       <c r="A23" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>66</v>
@@ -2312,7 +2839,7 @@
     </row>
     <row r="24" spans="1:3" ht="15.75">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>68</v>
@@ -2323,7 +2850,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75">
       <c r="A25" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>68</v>
@@ -2334,7 +2861,7 @@
     </row>
     <row r="26" spans="1:3" ht="15.75">
       <c r="A26" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>70</v>
@@ -2345,7 +2872,7 @@
     </row>
     <row r="27" spans="1:3" ht="15.75">
       <c r="A27" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>73</v>
@@ -2354,9 +2881,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5">
+    <row r="28" spans="1:3" ht="15.75">
       <c r="A28" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>79</v>
@@ -2365,9 +2892,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5">
+    <row r="29" spans="1:3" ht="15.75">
       <c r="A29" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>81</v>
@@ -2378,7 +2905,7 @@
     </row>
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>83</v>
@@ -2389,7 +2916,7 @@
     </row>
     <row r="31" spans="1:3" ht="15.75">
       <c r="A31" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>85</v>
@@ -2398,9 +2925,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5">
+    <row r="32" spans="1:3" ht="15.75">
       <c r="A32" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>87</v>
@@ -2411,7 +2938,7 @@
     </row>
     <row r="33" spans="1:3" ht="15.75">
       <c r="A33" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>92</v>
@@ -2422,7 +2949,7 @@
     </row>
     <row r="34" spans="1:3" ht="15.75">
       <c r="A34" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>95</v>
@@ -2431,9 +2958,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="31.5">
+    <row r="35" spans="1:3" ht="15.75">
       <c r="A35" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>96</v>
@@ -2442,14 +2969,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5">
+    <row r="36" spans="1:3" ht="15.75">
       <c r="A36" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2469,9 +2996,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5">
+    <row r="39" spans="1:3" ht="15.75">
       <c r="A39" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>108</v>
@@ -2480,9 +3007,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5">
+    <row r="40" spans="1:3" ht="15.75">
       <c r="A40" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>111</v>
@@ -2491,9 +3018,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5">
+    <row r="41" spans="1:3" ht="15.75">
       <c r="A41" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>113</v>
@@ -2504,68 +3031,68 @@
     </row>
     <row r="42" spans="1:3" ht="15.75">
       <c r="A42" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75">
       <c r="A43" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C43" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75">
       <c r="A44" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C44" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75">
       <c r="A45" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C45" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75">
+      <c r="A46" t="s">
+        <v>245</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75">
+      <c r="A47" t="s">
+        <v>244</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" t="s">
         <v>257</v>
-      </c>
-      <c r="C45" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="31.5">
-      <c r="A46" t="s">
-        <v>253</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="31.5">
-      <c r="A47" t="s">
-        <v>252</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C47" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2612,9 +3139,10 @@
     <hyperlink ref="C31" r:id="rId40" xr:uid="{726CB30E-E0E8-427E-B1A0-FE48119D38B7}"/>
     <hyperlink ref="C32" r:id="rId41" xr:uid="{3BBA6185-2783-4FB6-B279-61DBDF2D9B87}"/>
     <hyperlink ref="C46" r:id="rId42" xr:uid="{790FC2A5-3649-491D-BB97-65A5FE23E30B}"/>
+    <hyperlink ref="C36" r:id="rId43" xr:uid="{6BFFB149-C592-4D1E-AA46-516DEB935178}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId43"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId44"/>
 </worksheet>
 </file>
 

</xml_diff>